<commit_message>
added missing reviewer cells
</commit_message>
<xml_diff>
--- a/Petros/Feedback.xlsx
+++ b/Petros/Feedback.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="75">
   <si>
     <t>Author</t>
   </si>
@@ -355,8 +355,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -487,7 +493,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -525,6 +531,9 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -562,6 +571,9 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -891,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1333,6 +1345,12 @@
       </c>
     </row>
     <row r="26" spans="1:6">
+      <c r="A26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="C26" s="9" t="s">
         <v>63</v>
       </c>
@@ -1344,6 +1362,15 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="48">
+      <c r="A27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E27" s="10" t="s">
         <v>68</v>
       </c>
@@ -1352,6 +1379,15 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="32">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="D28" s="10" t="s">
         <v>69</v>
       </c>
@@ -1363,12 +1399,24 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="32">
+      <c r="A29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E29" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>73</v>
       </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Petros feedback updated for most rescent document
</commit_message>
<xml_diff>
--- a/Petros/Feedback.xlsx
+++ b/Petros/Feedback.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FAST BACKUP_DESKTOP\Career Related\Career Enhancement\Engineering Accelarator\Fall-2017\Petros\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="15825" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
   <si>
     <t>Author</t>
   </si>
@@ -312,6 +307,88 @@
   </si>
   <si>
     <t>Tolorance column is removed from the Major Components BOMt as it is not required  and found more redandant</t>
+  </si>
+  <si>
+    <t>b2c46de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow Diagram </t>
+  </si>
+  <si>
+    <t>Looks Great!</t>
+  </si>
+  <si>
+    <t>There stil are some issues with this. I think I have been a little unclaer about this so we should meet so I can explain things better</t>
+  </si>
+  <si>
+    <t>Hardware Block Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General </t>
+  </si>
+  <si>
+    <t>Old version are cluttering up the folder structure</t>
+  </si>
+  <si>
+    <t>remove all old versions and put them in the Archive Folder</t>
+  </si>
+  <si>
+    <t>In some blocks the text doubled up</t>
+  </si>
+  <si>
+    <t>Remove extra text</t>
+  </si>
+  <si>
+    <t>Arduino block is small which clutters up the signals</t>
+  </si>
+  <si>
+    <t>match the Flow Diagram Block structure</t>
+  </si>
+  <si>
+    <t>Device under test block should outside the device boundary</t>
+  </si>
+  <si>
+    <t>The connectors are acceible by the user so as per the Visual Grammar it should be inside the boundary but touch it</t>
+  </si>
+  <si>
+    <t>Major Components BOM</t>
+  </si>
+  <si>
+    <t>Munch Cleaner :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gray lines between items is unncessary </t>
+  </si>
+  <si>
+    <t>you can remove them</t>
+  </si>
+  <si>
+    <t>Add them</t>
+  </si>
+  <si>
+    <t>Missing manufactureer and MFG part number for NTR4003NT1GOSCT-ND?</t>
+  </si>
+  <si>
+    <t>Full BOM</t>
+  </si>
+  <si>
+    <t>Great collection of information!</t>
+  </si>
+  <si>
+    <t>Should be in the Realization folder</t>
+  </si>
+  <si>
+    <t>It is part of the Manufacturing package so it should be part of the Realziation folder not the Architecture folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Reference and Heat Sink and 
+Bidirectional Current/Power Monitor with I2C Interface are part of the major components BOM even if they are not part of the sub-functional </t>
+  </si>
+  <si>
+    <t>move them to the Major components BOM. Mark the subfunctional parts in another way</t>
+  </si>
+  <si>
+    <t>To be complete the Full BOM is generated from the schematic. We can talk about how to enter the information when we meet.</t>
   </si>
 </sst>
 </file>
@@ -321,7 +398,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -391,7 +468,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +487,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,7 +503,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -502,8 +585,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -554,8 +669,20 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -596,6 +723,22 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -636,6 +779,22 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -973,22 +1132,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="73" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="55" style="4" customWidth="1"/>
     <col min="6" max="6" width="66.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="67.125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="67.25" style="5" customWidth="1"/>
+    <col min="7" max="7" width="67.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="67.1640625" style="5" customWidth="1"/>
     <col min="9" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
@@ -1014,7 +1173,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="33.75">
+    <row r="3" spans="1:9" ht="32">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1184,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5">
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1035,7 +1194,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="16.5">
+    <row r="5" spans="1:9">
       <c r="A5" s="9"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1071,7 +1230,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="50.25">
+    <row r="7" spans="1:9" ht="48">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1250,7 @@
       <c r="G7" s="18"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="33.75">
+    <row r="8" spans="1:9" ht="32">
       <c r="A8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1151,14 +1310,16 @@
       <c r="G10" s="19"/>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12"/>
-      <c r="D11" s="14"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" spans="1:9" ht="34.5">
+    <row r="11" spans="1:9" s="27" customFormat="1">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="32">
       <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1371,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="34.5">
+    <row r="14" spans="1:9" ht="32">
       <c r="A14" s="10" t="s">
         <v>1</v>
       </c>
@@ -1236,7 +1397,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="34.5">
+    <row r="15" spans="1:9" ht="32">
       <c r="A15" s="10" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1447,7 @@
       </c>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="1:8" ht="172.5">
+    <row r="17" spans="1:8" ht="144">
       <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
@@ -1312,7 +1473,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="120.75">
+    <row r="18" spans="1:8" ht="112">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
@@ -1334,7 +1495,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
     </row>
-    <row r="19" spans="1:8" ht="34.5">
+    <row r="19" spans="1:8" ht="32">
       <c r="A19" s="10" t="s">
         <v>1</v>
       </c>
@@ -1358,7 +1519,7 @@
       </c>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="34.5">
+    <row r="20" spans="1:8" ht="32">
       <c r="A20" s="10" t="s">
         <v>1</v>
       </c>
@@ -1420,7 +1581,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="1:8" ht="34.5">
+    <row r="23" spans="1:8" ht="32">
       <c r="A23" s="10" t="s">
         <v>1</v>
       </c>
@@ -1439,7 +1600,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="1:8" ht="34.5">
+    <row r="24" spans="1:8" ht="32">
       <c r="A24" s="10" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1638,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="1:8" ht="34.5">
+    <row r="26" spans="1:8">
       <c r="A26" s="10" t="s">
         <v>1</v>
       </c>
@@ -1496,7 +1657,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="1:8" ht="51.75">
+    <row r="27" spans="1:8" ht="48">
       <c r="A27" s="10" t="s">
         <v>1</v>
       </c>
@@ -1519,7 +1680,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="34.5">
+    <row r="28" spans="1:8" ht="32">
       <c r="A28" s="10" t="s">
         <v>1</v>
       </c>
@@ -1545,7 +1706,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="34.5">
+    <row r="29" spans="1:8" ht="32">
       <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
@@ -1564,14 +1725,226 @@
       <c r="G29" s="19"/>
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="B30" s="16"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
+    <row r="30" spans="1:8" s="27" customFormat="1">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:8" customFormat="1">
+      <c r="A31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="1:6" ht="32">
+      <c r="A33" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="32">
+      <c r="A36" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="32">
+      <c r="A39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="32">
+      <c r="A41" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="32">
+      <c r="A42" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="64">
+      <c r="A43" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>